<commit_message>
Finalize Wars Analysis and Defense Analysis pages
</commit_message>
<xml_diff>
--- a/Data/WarsAnalysis/WarsAnalysis.xlsx
+++ b/Data/WarsAnalysis/WarsAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbbfilm/Documents/BasketballAnalyticsPortal/Data/WarsAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE7AE8B-ED0A-C242-91F9-B4242ED4B653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E48E1D2-7B1A-DB40-8DC8-04676C70C1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29200" windowHeight="18980" xr2:uid="{844EBB4D-025B-E04F-A75E-E177307491E4}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{844EBB4D-025B-E04F-A75E-E177307491E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Wars Analysis" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -507,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -530,7 +530,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2638,268 +2637,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C186F50-154B-A147-B546-F869F4B3C03D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AD1:AF4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="22">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="20" showAll="0">
-      <items count="67">
-        <item x="7"/>
-        <item x="10"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="64"/>
-        <item x="4"/>
-        <item x="56"/>
-        <item x="15"/>
-        <item x="41"/>
-        <item x="62"/>
-        <item x="12"/>
-        <item x="33"/>
-        <item x="23"/>
-        <item x="26"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="61"/>
-        <item x="53"/>
-        <item x="58"/>
-        <item x="63"/>
-        <item x="22"/>
-        <item x="14"/>
-        <item x="57"/>
-        <item x="39"/>
-        <item x="20"/>
-        <item x="65"/>
-        <item x="27"/>
-        <item x="32"/>
-        <item x="34"/>
-        <item x="19"/>
-        <item x="36"/>
-        <item x="6"/>
-        <item x="13"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="8"/>
-        <item x="49"/>
-        <item x="47"/>
-        <item x="52"/>
-        <item x="59"/>
-        <item x="5"/>
-        <item x="48"/>
-        <item x="60"/>
-        <item x="11"/>
-        <item x="2"/>
-        <item x="43"/>
-        <item x="46"/>
-        <item x="51"/>
-        <item x="37"/>
-        <item x="24"/>
-        <item x="44"/>
-        <item x="50"/>
-        <item x="30"/>
-        <item x="54"/>
-        <item x="31"/>
-        <item x="17"/>
-        <item x="25"/>
-        <item x="16"/>
-        <item x="45"/>
-        <item x="18"/>
-        <item x="21"/>
-        <item x="55"/>
-        <item x="38"/>
-        <item x="40"/>
-        <item x="42"/>
-        <item x="35"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="63">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item sd="0" x="14"/>
-        <item sd="0" x="15"/>
-        <item sd="0" x="16"/>
-        <item sd="0" x="17"/>
-        <item sd="0" x="18"/>
-        <item sd="0" x="19"/>
-        <item sd="0" x="20"/>
-        <item sd="0" x="21"/>
-        <item sd="0" x="22"/>
-        <item sd="0" x="23"/>
-        <item sd="0" x="24"/>
-        <item sd="0" x="25"/>
-        <item sd="0" x="26"/>
-        <item sd="0" x="27"/>
-        <item sd="0" x="28"/>
-        <item sd="0" x="29"/>
-        <item sd="0" x="30"/>
-        <item sd="0" x="31"/>
-        <item sd="0" x="32"/>
-        <item sd="0" x="33"/>
-        <item sd="0" x="34"/>
-        <item sd="0" x="35"/>
-        <item sd="0" x="36"/>
-        <item sd="0" x="37"/>
-        <item sd="0" x="38"/>
-        <item sd="0" x="39"/>
-        <item sd="0" x="40"/>
-        <item sd="0" x="41"/>
-        <item sd="0" x="42"/>
-        <item sd="0" x="43"/>
-        <item sd="0" x="44"/>
-        <item sd="0" x="45"/>
-        <item sd="0" x="46"/>
-        <item sd="0" x="47"/>
-        <item sd="0" x="48"/>
-        <item sd="0" x="49"/>
-        <item sd="0" x="50"/>
-        <item sd="0" x="51"/>
-        <item sd="0" x="52"/>
-        <item sd="0" x="53"/>
-        <item sd="0" x="54"/>
-        <item sd="0" x="55"/>
-        <item sd="0" x="56"/>
-        <item sd="0" x="57"/>
-        <item sd="0" x="58"/>
-        <item sd="0" x="59"/>
-        <item sd="0" x="60"/>
-        <item sd="0" x="61"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="27">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item sd="0" x="14"/>
-        <item sd="0" x="15"/>
-        <item sd="0" x="16"/>
-        <item sd="0" x="17"/>
-        <item sd="0" x="18"/>
-        <item sd="0" x="19"/>
-        <item sd="0" x="20"/>
-        <item sd="0" x="21"/>
-        <item sd="0" x="22"/>
-        <item sd="0" x="23"/>
-        <item sd="0" x="24"/>
-        <item sd="0" x="25"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count of Lineup" fld="12" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Average of Seconds" fld="19" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="7">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea field="4" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{557DDF41-715E-BB4F-9F61-77278B66C5BB}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{557DDF41-715E-BB4F-9F61-77278B66C5BB}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="V1:AA51" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="22">
     <pivotField showAll="0"/>
@@ -3347,6 +3085,267 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C186F50-154B-A147-B546-F869F4B3C03D}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AD1:AF4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="22">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="20" showAll="0">
+      <items count="67">
+        <item x="7"/>
+        <item x="10"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="64"/>
+        <item x="4"/>
+        <item x="56"/>
+        <item x="15"/>
+        <item x="41"/>
+        <item x="62"/>
+        <item x="12"/>
+        <item x="33"/>
+        <item x="23"/>
+        <item x="26"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="61"/>
+        <item x="53"/>
+        <item x="58"/>
+        <item x="63"/>
+        <item x="22"/>
+        <item x="14"/>
+        <item x="57"/>
+        <item x="39"/>
+        <item x="20"/>
+        <item x="65"/>
+        <item x="27"/>
+        <item x="32"/>
+        <item x="34"/>
+        <item x="19"/>
+        <item x="36"/>
+        <item x="6"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="49"/>
+        <item x="47"/>
+        <item x="52"/>
+        <item x="59"/>
+        <item x="5"/>
+        <item x="48"/>
+        <item x="60"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="43"/>
+        <item x="46"/>
+        <item x="51"/>
+        <item x="37"/>
+        <item x="24"/>
+        <item x="44"/>
+        <item x="50"/>
+        <item x="30"/>
+        <item x="54"/>
+        <item x="31"/>
+        <item x="17"/>
+        <item x="25"/>
+        <item x="16"/>
+        <item x="45"/>
+        <item x="18"/>
+        <item x="21"/>
+        <item x="55"/>
+        <item x="38"/>
+        <item x="40"/>
+        <item x="42"/>
+        <item x="35"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="63">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item sd="0" x="26"/>
+        <item sd="0" x="27"/>
+        <item sd="0" x="28"/>
+        <item sd="0" x="29"/>
+        <item sd="0" x="30"/>
+        <item sd="0" x="31"/>
+        <item sd="0" x="32"/>
+        <item sd="0" x="33"/>
+        <item sd="0" x="34"/>
+        <item sd="0" x="35"/>
+        <item sd="0" x="36"/>
+        <item sd="0" x="37"/>
+        <item sd="0" x="38"/>
+        <item sd="0" x="39"/>
+        <item sd="0" x="40"/>
+        <item sd="0" x="41"/>
+        <item sd="0" x="42"/>
+        <item sd="0" x="43"/>
+        <item sd="0" x="44"/>
+        <item sd="0" x="45"/>
+        <item sd="0" x="46"/>
+        <item sd="0" x="47"/>
+        <item sd="0" x="48"/>
+        <item sd="0" x="49"/>
+        <item sd="0" x="50"/>
+        <item sd="0" x="51"/>
+        <item sd="0" x="52"/>
+        <item sd="0" x="53"/>
+        <item sd="0" x="54"/>
+        <item sd="0" x="55"/>
+        <item sd="0" x="56"/>
+        <item sd="0" x="57"/>
+        <item sd="0" x="58"/>
+        <item sd="0" x="59"/>
+        <item sd="0" x="60"/>
+        <item sd="0" x="61"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="27">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Lineup" fld="12" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Average of Seconds" fld="19" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea field="4" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}" name="WarsAnalysis" displayName="WarsAnalysis" ref="A1:L182" totalsRowShown="0">
   <autoFilter ref="A1:L182" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}"/>
@@ -3739,8 +3738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F10F05-03F4-A745-9F0E-4F1A51D27D02}">
   <dimension ref="A1:L182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="L181" sqref="L181"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="L182" sqref="L182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10651,7 +10650,7 @@
         <f t="shared" ref="D173:D182" si="5">B173-C173</f>
         <v>10</v>
       </c>
-      <c r="E173" s="20">
+      <c r="E173">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>
@@ -10691,7 +10690,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E174" s="20">
+      <c r="E174">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -10731,7 +10730,7 @@
         <f t="shared" si="5"/>
         <v>-5</v>
       </c>
-      <c r="E175" s="20">
+      <c r="E175">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -10771,7 +10770,7 @@
         <f t="shared" si="5"/>
         <v>-6</v>
       </c>
-      <c r="E176" s="20">
+      <c r="E176">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -10811,7 +10810,7 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="E177" s="20">
+      <c r="E177">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>
@@ -10851,7 +10850,7 @@
         <f t="shared" si="5"/>
         <v>-5</v>
       </c>
-      <c r="E178" s="20">
+      <c r="E178">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -10891,7 +10890,7 @@
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
-      <c r="E179" s="20">
+      <c r="E179">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -10931,7 +10930,7 @@
         <f t="shared" si="5"/>
         <v>-8</v>
       </c>
-      <c r="E180" s="20">
+      <c r="E180">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -10971,7 +10970,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E181" s="20">
+      <c r="E181">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -11011,7 +11010,7 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="E182" s="20">
+      <c r="E182">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Add War Data for Lipscomb game
</commit_message>
<xml_diff>
--- a/Data/WarsAnalysis/WarsAnalysis.xlsx
+++ b/Data/WarsAnalysis/WarsAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbbfilm/Documents/BasketballAnalyticsPortal/Data/WarsAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E48E1D2-7B1A-DB40-8DC8-04676C70C1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00E5BC5-20AA-AE48-8DB9-4DA28A8BF01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{844EBB4D-025B-E04F-A75E-E177307491E4}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="105">
   <si>
     <t>WarNum</t>
   </si>
@@ -353,6 +353,9 @@
   <si>
     <t>UNA</t>
   </si>
+  <si>
+    <t>Lipscomb</t>
+  </si>
 </sst>
 </file>
 
@@ -507,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -530,11 +533,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -600,9 +607,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2637,7 +2641,268 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{557DDF41-715E-BB4F-9F61-77278B66C5BB}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C186F50-154B-A147-B546-F869F4B3C03D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AD1:AF4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="22">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="20" showAll="0">
+      <items count="67">
+        <item x="7"/>
+        <item x="10"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="64"/>
+        <item x="4"/>
+        <item x="56"/>
+        <item x="15"/>
+        <item x="41"/>
+        <item x="62"/>
+        <item x="12"/>
+        <item x="33"/>
+        <item x="23"/>
+        <item x="26"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="61"/>
+        <item x="53"/>
+        <item x="58"/>
+        <item x="63"/>
+        <item x="22"/>
+        <item x="14"/>
+        <item x="57"/>
+        <item x="39"/>
+        <item x="20"/>
+        <item x="65"/>
+        <item x="27"/>
+        <item x="32"/>
+        <item x="34"/>
+        <item x="19"/>
+        <item x="36"/>
+        <item x="6"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="49"/>
+        <item x="47"/>
+        <item x="52"/>
+        <item x="59"/>
+        <item x="5"/>
+        <item x="48"/>
+        <item x="60"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="43"/>
+        <item x="46"/>
+        <item x="51"/>
+        <item x="37"/>
+        <item x="24"/>
+        <item x="44"/>
+        <item x="50"/>
+        <item x="30"/>
+        <item x="54"/>
+        <item x="31"/>
+        <item x="17"/>
+        <item x="25"/>
+        <item x="16"/>
+        <item x="45"/>
+        <item x="18"/>
+        <item x="21"/>
+        <item x="55"/>
+        <item x="38"/>
+        <item x="40"/>
+        <item x="42"/>
+        <item x="35"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="63">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item sd="0" x="26"/>
+        <item sd="0" x="27"/>
+        <item sd="0" x="28"/>
+        <item sd="0" x="29"/>
+        <item sd="0" x="30"/>
+        <item sd="0" x="31"/>
+        <item sd="0" x="32"/>
+        <item sd="0" x="33"/>
+        <item sd="0" x="34"/>
+        <item sd="0" x="35"/>
+        <item sd="0" x="36"/>
+        <item sd="0" x="37"/>
+        <item sd="0" x="38"/>
+        <item sd="0" x="39"/>
+        <item sd="0" x="40"/>
+        <item sd="0" x="41"/>
+        <item sd="0" x="42"/>
+        <item sd="0" x="43"/>
+        <item sd="0" x="44"/>
+        <item sd="0" x="45"/>
+        <item sd="0" x="46"/>
+        <item sd="0" x="47"/>
+        <item sd="0" x="48"/>
+        <item sd="0" x="49"/>
+        <item sd="0" x="50"/>
+        <item sd="0" x="51"/>
+        <item sd="0" x="52"/>
+        <item sd="0" x="53"/>
+        <item sd="0" x="54"/>
+        <item sd="0" x="55"/>
+        <item sd="0" x="56"/>
+        <item sd="0" x="57"/>
+        <item sd="0" x="58"/>
+        <item sd="0" x="59"/>
+        <item sd="0" x="60"/>
+        <item sd="0" x="61"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="27">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Lineup" fld="12" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Average of Seconds" fld="19" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea field="4" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{557DDF41-715E-BB4F-9F61-77278B66C5BB}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="V1:AA51" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="22">
     <pivotField showAll="0"/>
@@ -3085,270 +3350,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C186F50-154B-A147-B546-F869F4B3C03D}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AD1:AF4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="22">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="20" showAll="0">
-      <items count="67">
-        <item x="7"/>
-        <item x="10"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="64"/>
-        <item x="4"/>
-        <item x="56"/>
-        <item x="15"/>
-        <item x="41"/>
-        <item x="62"/>
-        <item x="12"/>
-        <item x="33"/>
-        <item x="23"/>
-        <item x="26"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="61"/>
-        <item x="53"/>
-        <item x="58"/>
-        <item x="63"/>
-        <item x="22"/>
-        <item x="14"/>
-        <item x="57"/>
-        <item x="39"/>
-        <item x="20"/>
-        <item x="65"/>
-        <item x="27"/>
-        <item x="32"/>
-        <item x="34"/>
-        <item x="19"/>
-        <item x="36"/>
-        <item x="6"/>
-        <item x="13"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="8"/>
-        <item x="49"/>
-        <item x="47"/>
-        <item x="52"/>
-        <item x="59"/>
-        <item x="5"/>
-        <item x="48"/>
-        <item x="60"/>
-        <item x="11"/>
-        <item x="2"/>
-        <item x="43"/>
-        <item x="46"/>
-        <item x="51"/>
-        <item x="37"/>
-        <item x="24"/>
-        <item x="44"/>
-        <item x="50"/>
-        <item x="30"/>
-        <item x="54"/>
-        <item x="31"/>
-        <item x="17"/>
-        <item x="25"/>
-        <item x="16"/>
-        <item x="45"/>
-        <item x="18"/>
-        <item x="21"/>
-        <item x="55"/>
-        <item x="38"/>
-        <item x="40"/>
-        <item x="42"/>
-        <item x="35"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="63">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item sd="0" x="14"/>
-        <item sd="0" x="15"/>
-        <item sd="0" x="16"/>
-        <item sd="0" x="17"/>
-        <item sd="0" x="18"/>
-        <item sd="0" x="19"/>
-        <item sd="0" x="20"/>
-        <item sd="0" x="21"/>
-        <item sd="0" x="22"/>
-        <item sd="0" x="23"/>
-        <item sd="0" x="24"/>
-        <item sd="0" x="25"/>
-        <item sd="0" x="26"/>
-        <item sd="0" x="27"/>
-        <item sd="0" x="28"/>
-        <item sd="0" x="29"/>
-        <item sd="0" x="30"/>
-        <item sd="0" x="31"/>
-        <item sd="0" x="32"/>
-        <item sd="0" x="33"/>
-        <item sd="0" x="34"/>
-        <item sd="0" x="35"/>
-        <item sd="0" x="36"/>
-        <item sd="0" x="37"/>
-        <item sd="0" x="38"/>
-        <item sd="0" x="39"/>
-        <item sd="0" x="40"/>
-        <item sd="0" x="41"/>
-        <item sd="0" x="42"/>
-        <item sd="0" x="43"/>
-        <item sd="0" x="44"/>
-        <item sd="0" x="45"/>
-        <item sd="0" x="46"/>
-        <item sd="0" x="47"/>
-        <item sd="0" x="48"/>
-        <item sd="0" x="49"/>
-        <item sd="0" x="50"/>
-        <item sd="0" x="51"/>
-        <item sd="0" x="52"/>
-        <item sd="0" x="53"/>
-        <item sd="0" x="54"/>
-        <item sd="0" x="55"/>
-        <item sd="0" x="56"/>
-        <item sd="0" x="57"/>
-        <item sd="0" x="58"/>
-        <item sd="0" x="59"/>
-        <item sd="0" x="60"/>
-        <item sd="0" x="61"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="27">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item sd="0" x="14"/>
-        <item sd="0" x="15"/>
-        <item sd="0" x="16"/>
-        <item sd="0" x="17"/>
-        <item sd="0" x="18"/>
-        <item sd="0" x="19"/>
-        <item sd="0" x="20"/>
-        <item sd="0" x="21"/>
-        <item sd="0" x="22"/>
-        <item sd="0" x="23"/>
-        <item sd="0" x="24"/>
-        <item sd="0" x="25"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count of Lineup" fld="12" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Average of Seconds" fld="19" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="7">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea field="4" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}" name="WarsAnalysis" displayName="WarsAnalysis" ref="A1:L182" totalsRowShown="0">
-  <autoFilter ref="A1:L182" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}" name="WarsAnalysis" displayName="WarsAnalysis" ref="A1:L192" totalsRowShown="0">
+  <autoFilter ref="A1:L192" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K161">
     <sortCondition ref="K1:K161"/>
   </sortState>
@@ -3357,7 +3361,7 @@
     <tableColumn id="2" xr3:uid="{59583B98-5196-A141-9F75-194A211B3FD4}" name="BU_Score"/>
     <tableColumn id="3" xr3:uid="{3D4AD2AE-8D5B-E748-8542-C2D124DE7B2E}" name="Opp_Score"/>
     <tableColumn id="4" xr3:uid="{955168FD-82D4-4746-90C4-A1E7E2266446}" name="ScoreDiff"/>
-    <tableColumn id="7" xr3:uid="{3EF17A98-0B0D-AC49-BD8C-7D668AE27FB4}" name="WarWon" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{3EF17A98-0B0D-AC49-BD8C-7D668AE27FB4}" name="WarWon" dataDxfId="0">
       <calculatedColumnFormula>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{32A831B3-7B02-674A-BCB8-EC43F7FC1BBA}" name="GameWon"/>
@@ -3736,10 +3740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F10F05-03F4-A745-9F0E-4F1A51D27D02}">
-  <dimension ref="A1:L182"/>
+  <dimension ref="A1:L192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="L182" sqref="L182"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="K195" sqref="K195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10647,7 +10651,7 @@
         <v>6</v>
       </c>
       <c r="D173">
-        <f t="shared" ref="D173:D182" si="5">B173-C173</f>
+        <f t="shared" ref="D173:D192" si="5">B173-C173</f>
         <v>10</v>
       </c>
       <c r="E173">
@@ -11036,18 +11040,418 @@
         <v>1</v>
       </c>
     </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>1</v>
+      </c>
+      <c r="B183">
+        <v>2</v>
+      </c>
+      <c r="C183">
+        <v>9</v>
+      </c>
+      <c r="D183">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="E183" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183" t="s">
+        <v>104</v>
+      </c>
+      <c r="H183">
+        <v>1</v>
+      </c>
+      <c r="I183" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J183">
+        <v>1</v>
+      </c>
+      <c r="K183">
+        <v>19</v>
+      </c>
+      <c r="L183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>2</v>
+      </c>
+      <c r="B184">
+        <v>8</v>
+      </c>
+      <c r="C184">
+        <v>15</v>
+      </c>
+      <c r="D184">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="E184" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184" t="s">
+        <v>104</v>
+      </c>
+      <c r="H184">
+        <v>1</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J184">
+        <v>1</v>
+      </c>
+      <c r="K184">
+        <v>19</v>
+      </c>
+      <c r="L184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>3</v>
+      </c>
+      <c r="B185">
+        <v>4</v>
+      </c>
+      <c r="C185">
+        <v>5</v>
+      </c>
+      <c r="D185">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="E185" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+      <c r="G185" t="s">
+        <v>104</v>
+      </c>
+      <c r="H185">
+        <v>1</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J185">
+        <v>1</v>
+      </c>
+      <c r="K185">
+        <v>19</v>
+      </c>
+      <c r="L185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>4</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+      <c r="C186">
+        <v>11</v>
+      </c>
+      <c r="D186">
+        <f t="shared" si="5"/>
+        <v>-9</v>
+      </c>
+      <c r="E186" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+      <c r="G186" t="s">
+        <v>104</v>
+      </c>
+      <c r="H186">
+        <v>1</v>
+      </c>
+      <c r="I186" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J186">
+        <v>1</v>
+      </c>
+      <c r="K186">
+        <v>19</v>
+      </c>
+      <c r="L186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>5</v>
+      </c>
+      <c r="B187">
+        <v>11</v>
+      </c>
+      <c r="C187">
+        <v>9</v>
+      </c>
+      <c r="D187">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E187" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+      <c r="G187" t="s">
+        <v>104</v>
+      </c>
+      <c r="H187">
+        <v>1</v>
+      </c>
+      <c r="I187" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J187">
+        <v>1</v>
+      </c>
+      <c r="K187">
+        <v>19</v>
+      </c>
+      <c r="L187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>6</v>
+      </c>
+      <c r="B188">
+        <v>10</v>
+      </c>
+      <c r="C188">
+        <v>7</v>
+      </c>
+      <c r="D188">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E188" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+      <c r="G188" t="s">
+        <v>104</v>
+      </c>
+      <c r="H188">
+        <v>1</v>
+      </c>
+      <c r="I188" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J188">
+        <v>2</v>
+      </c>
+      <c r="K188">
+        <v>19</v>
+      </c>
+      <c r="L188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>7</v>
+      </c>
+      <c r="B189">
+        <v>5</v>
+      </c>
+      <c r="C189">
+        <v>4</v>
+      </c>
+      <c r="D189">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E189" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189" t="s">
+        <v>104</v>
+      </c>
+      <c r="H189">
+        <v>1</v>
+      </c>
+      <c r="I189" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J189">
+        <v>2</v>
+      </c>
+      <c r="K189">
+        <v>19</v>
+      </c>
+      <c r="L189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>8</v>
+      </c>
+      <c r="B190">
+        <v>9</v>
+      </c>
+      <c r="C190">
+        <v>5</v>
+      </c>
+      <c r="D190">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E190" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+      <c r="G190" t="s">
+        <v>104</v>
+      </c>
+      <c r="H190">
+        <v>1</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J190">
+        <v>2</v>
+      </c>
+      <c r="K190">
+        <v>19</v>
+      </c>
+      <c r="L190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>9</v>
+      </c>
+      <c r="B191">
+        <v>7</v>
+      </c>
+      <c r="C191">
+        <v>4</v>
+      </c>
+      <c r="D191">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E191" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+      <c r="G191" t="s">
+        <v>104</v>
+      </c>
+      <c r="H191">
+        <v>1</v>
+      </c>
+      <c r="I191" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J191">
+        <v>2</v>
+      </c>
+      <c r="K191">
+        <v>19</v>
+      </c>
+      <c r="L191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>10</v>
+      </c>
+      <c r="B192">
+        <v>13</v>
+      </c>
+      <c r="C192">
+        <v>12</v>
+      </c>
+      <c r="D192">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E192" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+      <c r="G192" t="s">
+        <v>104</v>
+      </c>
+      <c r="H192">
+        <v>1</v>
+      </c>
+      <c r="I192" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J192">
+        <v>2</v>
+      </c>
+      <c r="K192">
+        <v>19</v>
+      </c>
+      <c r="L192">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="I1 I2:I161 I166:I172 I177:I182" twoDigitTextYear="1"/>
+    <ignoredError sqref="I1 I2:I161 I166:I172 I177:I182 I187 I192" twoDigitTextYear="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -16925,18 +17329,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D1048444 O2:O1048444 D1048446:D1048473">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1048446:O1048473">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update Gitignore / update Defense grading to amend Shot Quality / update Wars Analysis data
</commit_message>
<xml_diff>
--- a/Data/WarsAnalysis/WarsAnalysis.xlsx
+++ b/Data/WarsAnalysis/WarsAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbbfilm/Documents/BasketballAnalyticsPortal/Data/WarsAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00E5BC5-20AA-AE48-8DB9-4DA28A8BF01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9059D894-61B2-7E48-B00E-DD8B44361A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{844EBB4D-025B-E04F-A75E-E177307491E4}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="18100" windowHeight="18980" xr2:uid="{844EBB4D-025B-E04F-A75E-E177307491E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Wars Analysis" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="12" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="106">
   <si>
     <t>WarNum</t>
   </si>
@@ -356,6 +356,9 @@
   <si>
     <t>Lipscomb</t>
   </si>
+  <si>
+    <t>EKU</t>
+  </si>
 </sst>
 </file>
 
@@ -540,9 +543,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -607,6 +607,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2641,7 +2644,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C186F50-154B-A147-B546-F869F4B3C03D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C186F50-154B-A147-B546-F869F4B3C03D}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AD1:AF4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="22">
     <pivotField showAll="0"/>
@@ -2869,7 +2872,7 @@
     <dataField name="Average of Seconds" fld="19" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="8">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2879,7 +2882,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="6">
       <pivotArea field="4" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2902,7 +2905,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{557DDF41-715E-BB4F-9F61-77278B66C5BB}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{557DDF41-715E-BB4F-9F61-77278B66C5BB}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="V1:AA51" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="22">
     <pivotField showAll="0"/>
@@ -3351,8 +3354,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}" name="WarsAnalysis" displayName="WarsAnalysis" ref="A1:L192" totalsRowShown="0">
-  <autoFilter ref="A1:L192" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}" name="WarsAnalysis" displayName="WarsAnalysis" ref="A1:L202" totalsRowShown="0">
+  <autoFilter ref="A1:L202" xr:uid="{E5420D39-36AD-864E-B0F5-B1AC94A7702F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K161">
     <sortCondition ref="K1:K161"/>
   </sortState>
@@ -3361,7 +3364,7 @@
     <tableColumn id="2" xr3:uid="{59583B98-5196-A141-9F75-194A211B3FD4}" name="BU_Score"/>
     <tableColumn id="3" xr3:uid="{3D4AD2AE-8D5B-E748-8542-C2D124DE7B2E}" name="Opp_Score"/>
     <tableColumn id="4" xr3:uid="{955168FD-82D4-4746-90C4-A1E7E2266446}" name="ScoreDiff"/>
-    <tableColumn id="7" xr3:uid="{3EF17A98-0B0D-AC49-BD8C-7D668AE27FB4}" name="WarWon" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{3EF17A98-0B0D-AC49-BD8C-7D668AE27FB4}" name="WarWon" dataDxfId="8">
       <calculatedColumnFormula>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{32A831B3-7B02-674A-BCB8-EC43F7FC1BBA}" name="GameWon"/>
@@ -3740,10 +3743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F10F05-03F4-A745-9F0E-4F1A51D27D02}">
-  <dimension ref="A1:L192"/>
+  <dimension ref="A1:L202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="K195" sqref="K195"/>
+      <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10651,7 +10654,7 @@
         <v>6</v>
       </c>
       <c r="D173">
-        <f t="shared" ref="D173:D192" si="5">B173-C173</f>
+        <f t="shared" ref="D173:D202" si="5">B173-C173</f>
         <v>10</v>
       </c>
       <c r="E173">
@@ -11054,7 +11057,7 @@
         <f t="shared" si="5"/>
         <v>-7</v>
       </c>
-      <c r="E183" s="20">
+      <c r="E183">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -11094,7 +11097,7 @@
         <f t="shared" si="5"/>
         <v>-7</v>
       </c>
-      <c r="E184" s="20">
+      <c r="E184">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -11134,7 +11137,7 @@
         <f t="shared" si="5"/>
         <v>-1</v>
       </c>
-      <c r="E185" s="20">
+      <c r="E185">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -11174,7 +11177,7 @@
         <f t="shared" si="5"/>
         <v>-9</v>
       </c>
-      <c r="E186" s="20">
+      <c r="E186">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>0</v>
       </c>
@@ -11214,7 +11217,7 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="E187" s="20">
+      <c r="E187">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>
@@ -11254,7 +11257,7 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="E188" s="20">
+      <c r="E188">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>
@@ -11294,7 +11297,7 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="E189" s="20">
+      <c r="E189">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>
@@ -11334,7 +11337,7 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="E190" s="20">
+      <c r="E190">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>
@@ -11374,7 +11377,7 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="E191" s="20">
+      <c r="E191">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>
@@ -11414,7 +11417,7 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="E192" s="20">
+      <c r="E192">
         <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
         <v>1</v>
       </c>
@@ -11440,12 +11443,412 @@
         <v>0</v>
       </c>
     </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>1</v>
+      </c>
+      <c r="B193">
+        <v>7</v>
+      </c>
+      <c r="C193">
+        <v>7</v>
+      </c>
+      <c r="D193">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E193" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+      <c r="G193" t="s">
+        <v>105</v>
+      </c>
+      <c r="H193">
+        <v>1</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J193">
+        <v>1</v>
+      </c>
+      <c r="K193">
+        <v>20</v>
+      </c>
+      <c r="L193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>2</v>
+      </c>
+      <c r="B194">
+        <v>2</v>
+      </c>
+      <c r="C194">
+        <v>6</v>
+      </c>
+      <c r="D194">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+      <c r="E194" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+      <c r="G194" t="s">
+        <v>105</v>
+      </c>
+      <c r="H194">
+        <v>1</v>
+      </c>
+      <c r="I194" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J194">
+        <v>1</v>
+      </c>
+      <c r="K194">
+        <v>20</v>
+      </c>
+      <c r="L194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>3</v>
+      </c>
+      <c r="B195">
+        <v>5</v>
+      </c>
+      <c r="C195">
+        <v>12</v>
+      </c>
+      <c r="D195">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="E195" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195" t="s">
+        <v>105</v>
+      </c>
+      <c r="H195">
+        <v>1</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J195">
+        <v>1</v>
+      </c>
+      <c r="K195">
+        <v>20</v>
+      </c>
+      <c r="L195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>4</v>
+      </c>
+      <c r="B196">
+        <v>2</v>
+      </c>
+      <c r="C196">
+        <v>8</v>
+      </c>
+      <c r="D196">
+        <f t="shared" si="5"/>
+        <v>-6</v>
+      </c>
+      <c r="E196" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+      <c r="G196" t="s">
+        <v>105</v>
+      </c>
+      <c r="H196">
+        <v>1</v>
+      </c>
+      <c r="I196" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J196">
+        <v>1</v>
+      </c>
+      <c r="K196">
+        <v>20</v>
+      </c>
+      <c r="L196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>5</v>
+      </c>
+      <c r="B197">
+        <v>8</v>
+      </c>
+      <c r="C197">
+        <v>7</v>
+      </c>
+      <c r="D197">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E197" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+      <c r="G197" t="s">
+        <v>105</v>
+      </c>
+      <c r="H197">
+        <v>1</v>
+      </c>
+      <c r="I197" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J197">
+        <v>1</v>
+      </c>
+      <c r="K197">
+        <v>20</v>
+      </c>
+      <c r="L197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>6</v>
+      </c>
+      <c r="B198">
+        <v>11</v>
+      </c>
+      <c r="C198">
+        <v>3</v>
+      </c>
+      <c r="D198">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E198" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+      <c r="G198" t="s">
+        <v>105</v>
+      </c>
+      <c r="H198">
+        <v>1</v>
+      </c>
+      <c r="I198" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J198">
+        <v>2</v>
+      </c>
+      <c r="K198">
+        <v>20</v>
+      </c>
+      <c r="L198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>7</v>
+      </c>
+      <c r="B199">
+        <v>8</v>
+      </c>
+      <c r="C199">
+        <v>15</v>
+      </c>
+      <c r="D199">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="E199" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="G199" t="s">
+        <v>105</v>
+      </c>
+      <c r="H199">
+        <v>1</v>
+      </c>
+      <c r="I199" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J199">
+        <v>2</v>
+      </c>
+      <c r="K199">
+        <v>20</v>
+      </c>
+      <c r="L199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>8</v>
+      </c>
+      <c r="B200">
+        <v>10</v>
+      </c>
+      <c r="C200">
+        <v>12</v>
+      </c>
+      <c r="D200">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="E200" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+      <c r="G200" t="s">
+        <v>105</v>
+      </c>
+      <c r="H200">
+        <v>1</v>
+      </c>
+      <c r="I200" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J200">
+        <v>2</v>
+      </c>
+      <c r="K200">
+        <v>20</v>
+      </c>
+      <c r="L200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>9</v>
+      </c>
+      <c r="B201">
+        <v>9</v>
+      </c>
+      <c r="C201">
+        <v>10</v>
+      </c>
+      <c r="D201">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="E201" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+      <c r="G201" t="s">
+        <v>105</v>
+      </c>
+      <c r="H201">
+        <v>1</v>
+      </c>
+      <c r="I201" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J201">
+        <v>2</v>
+      </c>
+      <c r="K201">
+        <v>20</v>
+      </c>
+      <c r="L201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>10</v>
+      </c>
+      <c r="B202">
+        <v>7</v>
+      </c>
+      <c r="C202">
+        <v>9</v>
+      </c>
+      <c r="D202">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="E202" s="20">
+        <f>IF(WarsAnalysis[[#This Row],[ScoreDiff]]&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F202">
+        <v>0</v>
+      </c>
+      <c r="G202" t="s">
+        <v>105</v>
+      </c>
+      <c r="H202">
+        <v>1</v>
+      </c>
+      <c r="I202" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J202">
+        <v>2</v>
+      </c>
+      <c r="K202">
+        <v>20</v>
+      </c>
+      <c r="L202">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17329,18 +17732,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D1048444 O2:O1048444 D1048446:D1048473">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1048446:O1048473">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>